<commit_message>
Fixed the issue of tha app restarting after running a job loading data from an Excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/data/BANK_TRANSACTION.xlsx
+++ b/src/main/resources/data/BANK_TRANSACTION.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>17/10/2018-09:44</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>amount</t>
+  </si>
+  <si>
+    <t>3600.12</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,6 +484,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>640338</v>
+      </c>
+      <c r="B5">
+        <v>33214561</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Handled the exceptions related to parsing data extracted from Excel File
</commit_message>
<xml_diff>
--- a/src/main/resources/data/BANK_TRANSACTION.xlsx
+++ b/src/main/resources/data/BANK_TRANSACTION.xlsx
@@ -404,7 +404,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,9 +488,6 @@
       <c r="A5">
         <v>640338</v>
       </c>
-      <c r="B5">
-        <v>33214561</v>
-      </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>

</xml_diff>